<commit_message>
up ! dates !
</commit_message>
<xml_diff>
--- a/IHT/comparison_outcomes.xlsx
+++ b/IHT/comparison_outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameliagelil/Documents/GitHub/dspp_capstone_msf/IHT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9271C382-F455-B84A-8145-FF1449EE551B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49364C32-2F5D-D941-A79C-9ED9CD7B43B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15980" xr2:uid="{B2738E5F-0524-2544-9EA9-F18B0AA84B02}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     </r>
   </si>
   <si>
-    <t>Counterfactual</t>
-  </si>
-  <si>
     <t>Scale-up</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Scale up</t>
+  </si>
+  <si>
+    <t>Baseline</t>
   </si>
 </sst>
 </file>
@@ -283,6 +283,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Baseline</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -371,6 +374,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Scale-up</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -583,6 +589,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -711,7 +748,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Counterfactual</c:v>
+                  <c:v>Baseline</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1203,6 +1240,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'90_target'!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'90_target'!$B$3:$I$3</c:f>
@@ -1269,6 +1339,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'90_target'!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'90_target'!$B$4:$I$4</c:f>
@@ -1335,6 +1438,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'90_target'!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'90_target'!$B$5:$I$5</c:f>
@@ -1394,6 +1530,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1611,7 +1748,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Standard</a:t>
+              <a:t>Baseline</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1677,6 +1814,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'90_target'!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'90_target'!$M$3:$T$3</c:f>
@@ -1743,6 +1913,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'90_target'!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'90_target'!$M$4:$T$4</c:f>
@@ -1809,6 +2012,39 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'90_target'!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2030</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'90_target'!$M$5:$T$5</c:f>
@@ -1868,6 +2104,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4745,7 +4982,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4756,10 +4993,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="23" x14ac:dyDescent="0.3">
@@ -5669,12 +5906,12 @@
     </row>
     <row r="38" spans="1:20" ht="23" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B39">
         <v>480136</v>
@@ -5703,7 +5940,7 @@
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40">
         <v>480136</v>
@@ -5732,7 +5969,7 @@
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41">
         <v>0</v>

</xml_diff>